<commit_message>
Commit post DB Connection. ON WORK su alcuni test, serve manutenzione per eliminare l'uso dei fogli Excel dal framework
</commit_message>
<xml_diff>
--- a/Data Files/ProductFamiliesList.xlsx
+++ b/Data Files/ProductFamiliesList.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" tabRatio="516" xr2:uid="{8D57AD91-8C36-424A-B9A7-5DA0D5B87C89}"/>
   </bookViews>
   <sheets>
-    <sheet name="Oggetti1" sheetId="1" r:id="rId1"/>
+    <sheet name="Intestazioni" sheetId="2" r:id="rId1"/>
+    <sheet name="Oggetti1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="81">
   <si>
     <t>CENTRAL-CORE</t>
   </si>
@@ -246,13 +247,34 @@
   </si>
   <si>
     <t>UNO-DM-6.0-TL-PLUS-US</t>
+  </si>
+  <si>
+    <t>Product Families</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Family Name</t>
+  </si>
+  <si>
+    <t>Reference Part Number</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Product Line Name</t>
+  </si>
+  <si>
+    <t>Models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,6 +310,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF323232"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -349,7 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,15 +419,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,11 +744,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91284E60-D613-4C38-9746-5872CEB286E5}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" style="19" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404540A2-9628-48E3-AF40-191A34537DAC}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -722,7 +814,7 @@
     <col min="4" max="4" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="16" customWidth="1"/>
     <col min="8" max="23" width="3.5703125" style="1" customWidth="1"/>
     <col min="24" max="49" width="3.42578125" style="1" customWidth="1"/>
     <col min="50" max="16384" width="44.85546875" style="1"/>
@@ -790,7 +882,7 @@
       <c r="A4" s="7">
         <v>116</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -799,19 +891,19 @@
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="16"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="16"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
@@ -912,7 +1004,7 @@
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -922,7 +1014,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -932,7 +1024,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -962,7 +1054,7 @@
       <c r="E14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -972,7 +1064,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -982,7 +1074,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1012,7 +1104,7 @@
       <c r="E18" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="16" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1022,7 +1114,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1032,7 +1124,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="17" t="s">
+      <c r="F20" s="16" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1062,7 +1154,7 @@
       <c r="E22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="16" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1092,7 +1184,7 @@
       <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1110,36 +1202,36 @@
       <c r="A26" s="7">
         <v>43</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="18" t="s">
         <v>43</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E26" s="17" t="s">
+      <c r="E26" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F26" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="17" t="s">
+      <c r="E27" s="17"/>
+      <c r="F27" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="14"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="8"/>
       <c r="E28" s="9"/>
       <c r="F28" s="10" t="s">
@@ -1150,7 +1242,7 @@
       <c r="A29" s="7">
         <v>113</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="7" t="s">
@@ -1159,10 +1251,10 @@
       <c r="D29" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E29" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F29" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1180,7 +1272,7 @@
       <c r="A31" s="7">
         <v>113</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1189,10 +1281,10 @@
       <c r="D31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="16" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1222,7 +1314,7 @@
       <c r="E33" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1232,7 +1324,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="17" t="s">
+      <c r="F34" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1242,7 +1334,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1252,7 +1344,7 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1262,7 +1354,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1292,7 +1384,7 @@
       <c r="E39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1302,7 +1394,7 @@
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1312,7 +1404,7 @@
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1322,7 +1414,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1332,7 +1424,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1342,7 +1434,7 @@
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="6"/>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="16" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1350,7 +1442,7 @@
       <c r="A45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="F45" s="17" t="s">
+      <c r="F45" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1360,7 +1452,7 @@
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="4"/>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1370,7 +1462,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="4"/>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1380,7 +1472,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
-      <c r="F48" s="17" t="s">
+      <c r="F48" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1390,7 +1482,7 @@
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="4"/>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1420,7 +1512,7 @@
       <c r="E51" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1430,7 +1522,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1440,7 +1532,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1450,7 +1542,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1460,7 +1552,7 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1490,7 +1582,7 @@
       <c r="E57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F57" s="16" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1500,7 +1592,7 @@
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
-      <c r="F58" s="17" t="s">
+      <c r="F58" s="16" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1510,7 +1602,7 @@
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="4"/>
-      <c r="F59" s="17" t="s">
+      <c r="F59" s="16" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1520,7 +1612,7 @@
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
-      <c r="F60" s="17" t="s">
+      <c r="F60" s="16" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1530,7 +1622,7 @@
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="4"/>
-      <c r="F61" s="17" t="s">
+      <c r="F61" s="16" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1560,7 +1652,7 @@
       <c r="E63" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="F63" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1570,7 +1662,7 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
-      <c r="F64" s="17" t="s">
+      <c r="F64" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1580,7 +1672,7 @@
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
-      <c r="F65" s="17" t="s">
+      <c r="F65" s="16" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1610,7 +1702,7 @@
       <c r="E67" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F67" s="17" t="s">
+      <c r="F67" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1620,7 +1712,7 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
-      <c r="F68" s="17" t="s">
+      <c r="F68" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1630,7 +1722,7 @@
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
-      <c r="F69" s="17" t="s">
+      <c r="F69" s="16" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1660,7 +1752,7 @@
       <c r="E71" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F71" s="17" t="s">
+      <c r="F71" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1670,7 +1762,7 @@
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="17" t="s">
+      <c r="F72" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1680,7 +1772,7 @@
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
       <c r="E73" s="4"/>
-      <c r="F73" s="17" t="s">
+      <c r="F73" s="16" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1710,7 +1802,7 @@
       <c r="E75" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F75" s="17" t="s">
+      <c r="F75" s="16" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1720,7 +1812,7 @@
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="4"/>
-      <c r="F76" s="17" t="s">
+      <c r="F76" s="16" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1730,7 +1822,7 @@
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="4"/>
-      <c r="F77" s="17" t="s">
+      <c r="F77" s="16" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>